<commit_message>
added custom scrollbar, show/hide btn to sidebar
</commit_message>
<xml_diff>
--- a/spreadsheets/test input file.xlsx
+++ b/spreadsheets/test input file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54029c2d16ad9025/Coding/HTML/Client Map/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54029c2d16ad9025/Coding/HTML/Client Map/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="8_{623C9B82-6348-4046-81B0-A07CCF8E108D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4F20693-D6AD-480A-81DC-0CEB988DE866}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{623C9B82-6348-4046-81B0-A07CCF8E108D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{624D039D-A45A-407F-93AF-BDCC7575B117}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1300" yWindow="1420" windowWidth="17890" windowHeight="9400" xr2:uid="{D219FE3D-C73F-4388-ABB5-67FF6D64FC26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D219FE3D-C73F-4388-ABB5-67FF6D64FC26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,20 +484,20 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="23.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="74.26953125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.54296875" style="1"/>
+    <col min="1" max="1" width="40.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="74.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -514,7 +514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -531,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -548,7 +548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -565,7 +565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -582,7 +582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>